<commit_message>
Modificacion  2.9 - Se modificaron los campos solicitados segun Don Alvaro (13 columnas). - Se modifico modal de analisis de consumo para que tomase los ultimos 13 meses.
</commit_message>
<xml_diff>
--- a/Copia de Contrato Anual Cantidades Ordenadas CA 9 May  2016.xlsx
+++ b/Copia de Contrato Anual Cantidades Ordenadas CA 9 May  2016.xlsx
@@ -2270,14 +2270,14 @@
   <dimension ref="A1:T300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.375" customWidth="1"/>
     <col min="2" max="2" width="38.5" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="10.875" style="56"/>
     <col min="9" max="15" width="10.875" style="87"/>
     <col min="16" max="16" width="12" style="87" customWidth="1"/>
@@ -6900,7 +6900,7 @@
         <v>1040088</v>
       </c>
       <c r="R101" s="71">
-        <f t="shared" ref="R101:R132" si="6">Q101/E101</f>
+        <f t="shared" ref="R101:R102" si="6">Q101/E101</f>
         <v>0.57463425414364644</v>
       </c>
       <c r="S101" s="85">

</xml_diff>